<commit_message>
big picture dataset handling
</commit_message>
<xml_diff>
--- a/logs/result.xlsx
+++ b/logs/result.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:S13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -659,6 +659,625 @@
         <v>0.0012</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>resnet</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2025-09-26 16:27:11</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>uliege</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>/home/labsig/Documents/Axelle/Main research/Data/our/validation</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>all</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>0.8184</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.945</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.9458</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.9293</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.9664</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.9671999999999999</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.843</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.9452</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.9461000000000001</v>
+      </c>
+      <c r="O5" t="n">
+        <v>399.3357</v>
+      </c>
+      <c r="P5" t="n">
+        <v>313.5957</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>76.73990000000001</v>
+      </c>
+      <c r="R5" t="n">
+        <v>2.4342</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>hoptim</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2025-09-26 17:15:11</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>uliege</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>/home/labsig/Documents/Axelle/Main research/Data/our/validation</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>all</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>0.7585</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.906</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.9173</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.8879</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.9405</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.9506</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.7842</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.9192</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.9314</v>
+      </c>
+      <c r="O6" t="n">
+        <v>1772.5035</v>
+      </c>
+      <c r="P6" t="n">
+        <v>1624.6798</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>139.8535</v>
+      </c>
+      <c r="R6" t="n">
+        <v>2.4627</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>uni2</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2025-09-26 18:08:42</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>uliege</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>/home/labsig/Documents/Axelle/Main research/Data/our/validation</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>all</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>0.7889</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.9185</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.9304</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.9016999999999999</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.9415</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.9517</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.7988</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.9177</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.9308999999999999</v>
+      </c>
+      <c r="O7" t="n">
+        <v>1629.0576</v>
+      </c>
+      <c r="P7" t="n">
+        <v>1483.1252</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>138.4627</v>
+      </c>
+      <c r="R7" t="n">
+        <v>2.3626</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>hoptim</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2025-10-16 13:29:44</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>uliege</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>/home/labsig/Documents/Axelle/Main research/Data/uliege/sub_fold_test/val</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>all</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>0.7399</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.8786</v>
+      </c>
+      <c r="J8" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" t="n">
+        <v>1</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.7457</v>
+      </c>
+      <c r="M8" t="n">
+        <v>1</v>
+      </c>
+      <c r="N8" t="n">
+        <v>1</v>
+      </c>
+      <c r="O8" t="n">
+        <v>2.9859</v>
+      </c>
+      <c r="P8" t="n">
+        <v>2.8889</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0.0835</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0.0041</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>hoptim</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2025-10-16 13:47:10</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>uliege</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>/home/labsig/Documents/Axelle/Main research/Data/uliege/sub_fold_test/val</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>all</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>cells_no_aug_1</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>0.3654</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.5962</v>
+      </c>
+      <c r="K9" t="n">
+        <v>1</v>
+      </c>
+      <c r="L9" t="n">
+        <v>1</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.2692</v>
+      </c>
+      <c r="N9" t="n">
+        <v>1</v>
+      </c>
+      <c r="O9" t="n">
+        <v>1</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0.8982</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0.8682</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0.0258</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0.0012</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>hoptim</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2025-10-16 13:48:04</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>uliege</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>/home/labsig/Documents/Axelle/Main research/Data/uliege/sub_fold_test/val</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>all</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>cells_no_aug_0</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>0.9008</v>
+      </c>
+      <c r="H10" t="n">
+        <v>1</v>
+      </c>
+      <c r="I10" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" t="n">
+        <v>1</v>
+      </c>
+      <c r="K10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L10" t="n">
+        <v>1</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.9504</v>
+      </c>
+      <c r="N10" t="n">
+        <v>1</v>
+      </c>
+      <c r="O10" t="n">
+        <v>1</v>
+      </c>
+      <c r="P10" t="n">
+        <v>2.1195</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>2.054</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0.0553</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0.0031</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>hoptim1</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>2025-10-16 14:22:33</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>uliege</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>/home/labsig/Documents/Axelle/Main research/Data/uliege/sub_fold_test/val</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>all</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>cells_no_aug_0</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>0.8843</v>
+      </c>
+      <c r="H11" t="n">
+        <v>1</v>
+      </c>
+      <c r="I11" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.9917</v>
+      </c>
+      <c r="K11" t="n">
+        <v>1</v>
+      </c>
+      <c r="L11" t="n">
+        <v>1</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.9174</v>
+      </c>
+      <c r="N11" t="n">
+        <v>1</v>
+      </c>
+      <c r="O11" t="n">
+        <v>1</v>
+      </c>
+      <c r="P11" t="n">
+        <v>2.1013</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>2.0305</v>
+      </c>
+      <c r="R11" t="n">
+        <v>0.0604</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0.0031</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>hoptim1</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2025-10-16 14:23:14</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>uliege</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>/home/labsig/Documents/Axelle/Main research/Data/uliege/sub_fold_test/val</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>all</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>cells_no_aug_1</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>0.3846</v>
+      </c>
+      <c r="H12" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.5385</v>
+      </c>
+      <c r="K12" t="n">
+        <v>1</v>
+      </c>
+      <c r="L12" t="n">
+        <v>1</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.3654</v>
+      </c>
+      <c r="N12" t="n">
+        <v>1</v>
+      </c>
+      <c r="O12" t="n">
+        <v>1</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0.9251</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0.8939</v>
+      </c>
+      <c r="R12" t="n">
+        <v>0.0266</v>
+      </c>
+      <c r="S12" t="n">
+        <v>0.0013</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>uni2</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>2025-10-16 14:25:33</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>uliege</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>/home/labsig/Documents/Axelle/Main research/Data/uliege/sub_fold_test/val</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>all</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>cells_no_aug_1</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>0.2308</v>
+      </c>
+      <c r="H13" t="n">
+        <v>1</v>
+      </c>
+      <c r="I13" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.6731</v>
+      </c>
+      <c r="K13" t="n">
+        <v>1</v>
+      </c>
+      <c r="L13" t="n">
+        <v>1</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0.2308</v>
+      </c>
+      <c r="N13" t="n">
+        <v>1</v>
+      </c>
+      <c r="O13" t="n">
+        <v>1</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0.773</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0.7409</v>
+      </c>
+      <c r="R13" t="n">
+        <v>0.0272</v>
+      </c>
+      <c r="S13" t="n">
+        <v>0.0014</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>